<commit_message>
Company excel change 2 title
</commit_message>
<xml_diff>
--- a/backend/excel/company.xlsx
+++ b/backend/excel/company.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dir\ak\backend\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Tiny PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,16 +30,16 @@
     <t>Street Address</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
     <t>Contact Person</t>
   </si>
   <si>
     <t>Contact Mobile</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,16 +487,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>